<commit_message>
Correction du plan d'adressage IP
</commit_message>
<xml_diff>
--- a/Projet réseau Excel.xlsx
+++ b/Projet réseau Excel.xlsx
@@ -30,7 +30,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="247">
   <si>
-    <t>Nom de l'élément (classé par catégorie)</t>
+    <t>Colonne 1</t>
   </si>
   <si>
     <t>Poe(w)</t>
@@ -1974,7 +1974,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:P60" displayName="Répartition_des_équipements" name="Répartition_des_équipements" id="1">
   <tableColumns count="16">
-    <tableColumn name="Nom de l'élément (classé par catégorie)" id="1"/>
+    <tableColumn name="Colonne 1" id="1"/>
     <tableColumn name="Poe(w)" id="2"/>
     <tableColumn name="Bande passante" id="3"/>
     <tableColumn name="Sous-sol 5" id="4"/>
@@ -4279,7 +4279,7 @@
         <v>127</v>
       </c>
       <c r="V38" s="59" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="W38" s="59" t="s">
         <v>128</v>
@@ -4525,7 +4525,7 @@
         <v>150</v>
       </c>
       <c r="V44" s="59" t="s">
-        <v>142</v>
+        <v>99</v>
       </c>
       <c r="W44" s="59" t="s">
         <v>151</v>
@@ -11316,6 +11316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11612,6 +11613,9 @@
     </dataValidation>
     <dataValidation allowBlank="1" showDropDown="1" sqref="A2:A11 C2:C11"/>
   </dataValidations>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>

</xml_diff>